<commit_message>
Update aioquic, picoquic, lsquic
</commit_message>
<xml_diff>
--- a/Throughput553.xlsx
+++ b/Throughput553.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicod\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicod\Desktop\Statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C93185E-FB94-47A8-814B-EEAFBCB182FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B104D7-3520-487C-A62E-2D2914B71FF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10140" yWindow="0" windowWidth="10455" windowHeight="10905" xr2:uid="{B7222400-D840-4912-9CB9-AD244D6527CA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{B7222400-D840-4912-9CB9-AD244D6527CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Aioquic</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>Ngtpc2</t>
+  </si>
+  <si>
+    <t>Lsquic</t>
   </si>
 </sst>
 </file>
@@ -399,15 +402,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CB320D5-EF20-45ED-903F-FD8B3E360C19}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -420,341 +423,862 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>5.08</v>
+        <v>5.0815184877164636</v>
       </c>
       <c r="B2">
         <v>4.91</v>
       </c>
       <c r="C2">
-        <v>5.44</v>
+        <v>4.6380844711134301</v>
       </c>
       <c r="D2">
-        <v>1.37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.371781315195336</v>
+      </c>
+      <c r="E2">
+        <v>4.8236996599999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>5.0599999999999996</v>
+        <v>5.0643719957895046</v>
       </c>
       <c r="B3">
         <v>4.88</v>
       </c>
       <c r="C3">
-        <v>5.44</v>
+        <v>5.4392679582138701</v>
       </c>
       <c r="D3">
-        <v>1.39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.391612058318485</v>
+      </c>
+      <c r="E3">
+        <v>5.0014634960000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>5.0599999999999996</v>
+        <v>5.0670276432871457</v>
       </c>
       <c r="B4">
         <v>4.88</v>
       </c>
       <c r="C4">
-        <v>5.44</v>
+        <v>5.4399450984002371</v>
       </c>
       <c r="D4">
-        <v>1.38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.375681392189569</v>
+      </c>
+      <c r="E4">
+        <v>5.0101840529999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>5.43</v>
+        <v>5.4387673243042816</v>
       </c>
       <c r="B5">
         <v>5.44</v>
       </c>
       <c r="C5">
-        <v>5.44</v>
+        <v>5.4387673243042816</v>
       </c>
       <c r="D5">
-        <v>1.38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.363960193471258</v>
+      </c>
+      <c r="E5">
+        <v>5.0062863030000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5.43</v>
+        <v>5.4387673243042816</v>
       </c>
       <c r="B6">
         <v>5.44</v>
       </c>
       <c r="C6">
-        <v>5.44</v>
+        <v>5.4387673243042816</v>
       </c>
       <c r="D6">
-        <v>1.36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.3598113423644771</v>
+      </c>
+      <c r="E6">
+        <v>4.9962811770000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>5.07</v>
+        <v>5.0761271510826624</v>
       </c>
       <c r="B7">
         <v>4.87</v>
       </c>
       <c r="C7">
-        <v>5.38</v>
+        <v>5.4387673243042816</v>
       </c>
       <c r="D7">
-        <v>1.37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.3665730537010341</v>
+      </c>
+      <c r="E7">
+        <v>4.9952885350000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>4.75</v>
+        <v>4.7513418397085108</v>
       </c>
       <c r="B8">
         <v>4.88</v>
       </c>
       <c r="C8">
-        <v>5.04</v>
+        <v>5.3835914022362932</v>
       </c>
       <c r="D8">
-        <v>1.36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.3606770016024401</v>
+      </c>
+      <c r="E8">
+        <v>5.0018117359999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>4.7699999999999996</v>
+        <v>4.768545344153126</v>
       </c>
       <c r="B9">
         <v>5.08</v>
       </c>
       <c r="C9">
-        <v>5.01</v>
+        <v>5.0465226304999211</v>
       </c>
       <c r="D9">
-        <v>1.37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.3704172594265129</v>
+      </c>
+      <c r="E9">
+        <v>5.0071266210000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>4.76</v>
+        <v>4.7557296865365846</v>
       </c>
       <c r="B10">
         <v>4.79</v>
       </c>
       <c r="C10">
-        <v>5.0199999999999996</v>
+        <v>5.0152365065606919</v>
       </c>
       <c r="D10">
-        <v>1.35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.3547414742006421</v>
+      </c>
+      <c r="E10">
+        <v>4.9977212099999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>4.7699999999999996</v>
+        <v>4.7720513161983398</v>
       </c>
       <c r="B11">
         <v>5.07</v>
       </c>
       <c r="C11">
-        <v>5.04</v>
+        <v>5.0278169437431002</v>
       </c>
       <c r="D11">
-        <v>1.27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.370090356643491</v>
+      </c>
+      <c r="E11">
+        <v>5.0049196079999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>4.76</v>
+        <v>4.767857984360317</v>
       </c>
       <c r="B12">
         <v>4.9800000000000004</v>
       </c>
       <c r="C12">
-        <v>5.04</v>
+        <v>5.0469655805176163</v>
       </c>
       <c r="D12">
-        <v>1.26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.2629043643118261</v>
+      </c>
+      <c r="E12">
+        <v>5.0011579389999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>4.7699999999999996</v>
+        <v>4.7671906418939054</v>
       </c>
       <c r="B13">
         <v>5.07</v>
       </c>
       <c r="C13">
-        <v>5</v>
+        <v>5.0413099734372286</v>
       </c>
       <c r="D13">
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.3014413075147</v>
+      </c>
+      <c r="E13">
+        <v>5.0109258109999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>4.75</v>
+        <v>4.7510662276534159</v>
       </c>
       <c r="B14">
         <v>5.08</v>
       </c>
       <c r="C14">
-        <v>5.04</v>
+        <v>5.0094676215510567</v>
       </c>
       <c r="D14">
-        <v>1.33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.330130990191472</v>
+      </c>
+      <c r="E14">
+        <v>4.9948136239999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>4.7300000000000004</v>
+        <v>4.7339297534365716</v>
       </c>
       <c r="B15">
         <v>5.09</v>
       </c>
       <c r="C15">
-        <v>5.04</v>
+        <v>5.0651240060726428</v>
       </c>
       <c r="D15">
-        <v>1.38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.37646925803391</v>
+      </c>
+      <c r="E15">
+        <v>5.0008666269999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>4.7300000000000004</v>
+        <v>4.7333630544501863</v>
       </c>
       <c r="B16">
         <v>5.0599999999999996</v>
       </c>
       <c r="C16">
-        <v>5.05</v>
+        <v>5.0594485201113084</v>
       </c>
       <c r="D16">
-        <v>1.34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.344227443283404</v>
+      </c>
+      <c r="E16">
+        <v>4.9995525970000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>4.75</v>
+        <v>4.751571540849012</v>
       </c>
       <c r="B17">
         <v>5.07</v>
       </c>
       <c r="C17">
-        <v>5.04</v>
+        <v>5.0499228788951651</v>
       </c>
       <c r="D17">
-        <v>1.37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.115379725384217</v>
+      </c>
+      <c r="E17">
+        <v>4.9862594549999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>4.7300000000000004</v>
+        <v>4.7297185817443861</v>
       </c>
       <c r="B18">
         <v>5.08</v>
       </c>
       <c r="C18">
-        <v>4.9800000000000004</v>
+        <v>5.0607426639859403</v>
       </c>
       <c r="D18">
-        <v>1.37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.0999382266835189</v>
+      </c>
+      <c r="E18">
+        <v>5.0034825380000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>4.75</v>
+        <v>4.7506266269860449</v>
       </c>
       <c r="B19">
         <v>5.08</v>
       </c>
       <c r="C19">
-        <v>5.01</v>
+        <v>5.0265395826333057</v>
       </c>
       <c r="D19">
-        <v>1.37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.1100689531223831</v>
+      </c>
+      <c r="E19">
+        <v>5.0046634360000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>4.75</v>
+        <v>4.7495443751035511</v>
       </c>
       <c r="B20">
         <v>5.07</v>
       </c>
       <c r="C20">
-        <v>4.99</v>
+        <v>5.0426639516671621</v>
       </c>
       <c r="D20">
-        <v>1.38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.117978322533419</v>
+      </c>
+      <c r="E20">
+        <v>5.0130238929999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>4.75</v>
+        <v>4.7502199048022788</v>
       </c>
       <c r="B21">
         <v>5.09</v>
       </c>
       <c r="C21">
-        <v>5.04</v>
+        <v>4.9793519265220851</v>
       </c>
       <c r="D21">
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.123872865895877</v>
+      </c>
+      <c r="E21">
+        <v>4.990196815</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>4.74</v>
+        <v>4.7422569558846037</v>
       </c>
       <c r="B22">
         <v>4.91</v>
       </c>
       <c r="C22">
-        <v>5.04</v>
+        <v>5.0233901604345226</v>
       </c>
       <c r="D22">
-        <v>1.33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.115379725384217</v>
+      </c>
+      <c r="E22">
+        <v>5.0061795030000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>4.76</v>
+        <v>4.7597699813483434</v>
       </c>
       <c r="B23">
         <v>5.07</v>
       </c>
       <c r="C23">
-        <v>5.4</v>
+        <v>5.0442260745366641</v>
       </c>
       <c r="D23">
-        <v>1.38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.0999382266835189</v>
+      </c>
+      <c r="E23">
+        <v>5.0140378820000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>4.76</v>
+        <v>4.7642196028247392</v>
       </c>
       <c r="B24">
         <v>4.9800000000000004</v>
       </c>
       <c r="C24">
-        <v>4.97</v>
+        <v>5.0367560006514944</v>
       </c>
       <c r="D24">
-        <v>1.37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.1100689531223831</v>
+      </c>
+      <c r="E24">
+        <v>4.992688265</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>4.76</v>
+        <v>4.7592365852477503</v>
       </c>
       <c r="B25">
         <v>5.09</v>
       </c>
       <c r="C25">
-        <v>4.9800000000000004</v>
+        <v>5.0461281935958064</v>
       </c>
       <c r="D25">
-        <v>1.37</v>
+        <v>1.117978322533419</v>
+      </c>
+      <c r="E25">
+        <v>5.0036532349999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>4.7365370131452664</v>
+      </c>
+      <c r="B26">
+        <v>4.9512273909999998</v>
+      </c>
+      <c r="C26">
+        <v>5.0570637423645897</v>
+      </c>
+      <c r="D26">
+        <v>1.123872865895877</v>
+      </c>
+      <c r="E26">
+        <v>4.997245836101694</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>4.7270733507117404</v>
+      </c>
+      <c r="B27">
+        <v>5.0639397749999997</v>
+      </c>
+      <c r="E27">
+        <v>4.968361979045369</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>4.7148476583380159</v>
+      </c>
+      <c r="B28">
+        <v>4.7818360210000002</v>
+      </c>
+      <c r="E28">
+        <v>4.9833581321467664</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>4.7398719683420643</v>
+      </c>
+      <c r="B29">
+        <v>4.9368147909999998</v>
+      </c>
+      <c r="E29">
+        <v>4.9676748318117481</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>4.7165607497137847</v>
+      </c>
+      <c r="B30">
+        <v>4.9327758900000003</v>
+      </c>
+      <c r="E30">
+        <v>4.97074743378103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>4.741237325115188</v>
+      </c>
+      <c r="B31">
+        <v>4.9352251699999998</v>
+      </c>
+      <c r="E31">
+        <v>4.9607788422782377</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>4.7332914125159782</v>
+      </c>
+      <c r="B32">
+        <v>4.9288769070000003</v>
+      </c>
+      <c r="E32">
+        <v>4.9716390590043167</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>4.712173846339299</v>
+      </c>
+      <c r="B33">
+        <v>5.0508922490000003</v>
+      </c>
+      <c r="E33">
+        <v>4.9718075910462263</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>4.719511475684226</v>
+      </c>
+      <c r="B34">
+        <v>4.8952831909999999</v>
+      </c>
+      <c r="E34">
+        <v>4.9625342760268714</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>4.7303169312343929</v>
+      </c>
+      <c r="B35">
+        <v>4.9130627550000003</v>
+      </c>
+      <c r="E35">
+        <v>4.9992827733521183</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>4.7433555103588549</v>
+      </c>
+      <c r="B36">
+        <v>4.7872938219999996</v>
+      </c>
+      <c r="E36">
+        <v>4.9535952265355094</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>4.7050777910753974</v>
+      </c>
+      <c r="B37">
+        <v>5.0680414730000001</v>
+      </c>
+      <c r="E37">
+        <v>4.9768759075375639</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>4.7095997798535922</v>
+      </c>
+      <c r="B38">
+        <v>4.9458146799999998</v>
+      </c>
+      <c r="E38">
+        <v>4.9663011074004926</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>4.7198028659082052</v>
+      </c>
+      <c r="B39">
+        <v>5.0458102509999998</v>
+      </c>
+      <c r="E39">
+        <v>4.9807420739696786</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>4.7418778111822846</v>
+      </c>
+      <c r="B40">
+        <v>4.9491355610000003</v>
+      </c>
+      <c r="E40">
+        <v>4.9974019188887597</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>4.713032493892924</v>
+      </c>
+      <c r="B41">
+        <v>4.9384574849999998</v>
+      </c>
+      <c r="E41">
+        <v>4.9624503226297607</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>4.7326402216636607</v>
+      </c>
+      <c r="B42">
+        <v>5.0617655920000004</v>
+      </c>
+      <c r="E42">
+        <v>4.9671771193759424</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>4.7217723117467809</v>
+      </c>
+      <c r="B43">
+        <v>4.9424014349999998</v>
+      </c>
+      <c r="E43">
+        <v>4.9819827725300261</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>4.7328160255351932</v>
+      </c>
+      <c r="B44">
+        <v>4.8507247209999997</v>
+      </c>
+      <c r="E44">
+        <v>4.9781428415861599</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>4.7384747621120384</v>
+      </c>
+      <c r="B45">
+        <v>4.8766611129999999</v>
+      </c>
+      <c r="E45">
+        <v>4.9724818334896659</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>4.7252747252747254</v>
+      </c>
+      <c r="B46">
+        <v>4.9220648059999998</v>
+      </c>
+      <c r="E46">
+        <v>4.9695193401833642</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>4.7018944260681774</v>
+      </c>
+      <c r="B47">
+        <v>4.9022325579999997</v>
+      </c>
+      <c r="E47">
+        <v>4.9637799184078668</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>4.6947652003259037</v>
+      </c>
+      <c r="B48">
+        <v>5.0719890349999996</v>
+      </c>
+      <c r="E48">
+        <v>4.9786427540946514</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>4.7198870520051974</v>
+      </c>
+      <c r="B49">
+        <v>4.9433474300000002</v>
+      </c>
+      <c r="E49">
+        <v>4.9689090280277517</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>4.723360726079405</v>
+      </c>
+      <c r="B50">
+        <v>5.0415326260000004</v>
+      </c>
+      <c r="E50">
+        <v>4.9665113220937789</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>4.7161598394312083</v>
+      </c>
+      <c r="B51">
+        <v>4.918241729</v>
+      </c>
+      <c r="E51">
+        <v>4.9742877371088916</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>4.7538040797036061</v>
+      </c>
+      <c r="B52">
+        <v>4.8894632070000004</v>
+      </c>
+      <c r="E52">
+        <v>4.9542854569202364</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>4.7108187238611192</v>
+      </c>
+      <c r="B53">
+        <v>4.9461080309999996</v>
+      </c>
+      <c r="E53">
+        <v>4.9730578937404459</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>4.734926691222217</v>
+      </c>
+      <c r="B54">
+        <v>4.9326794530000004</v>
+      </c>
+      <c r="E54">
+        <v>4.9617648095288436</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>4.7399699342604764</v>
+      </c>
+      <c r="B55">
+        <v>4.9463740669999998</v>
+      </c>
+      <c r="E55">
+        <v>4.9717724792619178</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>4.7197057318356492</v>
+      </c>
+      <c r="B56">
+        <v>5.0632072099999998</v>
+      </c>
+      <c r="E56">
+        <v>4.9850236859435073</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>4.7078273103251957</v>
+      </c>
+      <c r="B57">
+        <v>4.9312036949999998</v>
+      </c>
+      <c r="E57">
+        <v>4.9625482685358939</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>4.7363022421709893</v>
+      </c>
+      <c r="B58">
+        <v>4.9218949299999997</v>
+      </c>
+      <c r="E58">
+        <v>4.9683409411053994</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>4.7230040502505668</v>
+      </c>
+      <c r="B59">
+        <v>4.9103711130000001</v>
+      </c>
+      <c r="E59">
+        <v>4.9662870937203278</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>4.7199453364470338</v>
+      </c>
+      <c r="B60">
+        <v>5.0563725340000003</v>
+      </c>
+      <c r="E60">
+        <v>4.9780865197094037</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>4.7449388468419258</v>
+      </c>
+      <c r="B61">
+        <v>4.9402054399999997</v>
+      </c>
+      <c r="E61">
+        <v>4.9827232564361346</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>4.7203080275424476</v>
+      </c>
+      <c r="B62">
+        <v>4.904672723</v>
+      </c>
+      <c r="E62">
+        <v>4.9473361686816757</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>4.7098577047932384</v>
+      </c>
+      <c r="B63">
+        <v>4.9345940620000004</v>
+      </c>
+      <c r="E63">
+        <v>4.9794949490662743</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>4.7368435547256897</v>
+      </c>
+      <c r="B64">
+        <v>4.9361758480000004</v>
+      </c>
+      <c r="E64">
+        <v>4.9706421448320857</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>4.7267096192662894</v>
+      </c>
+      <c r="B65">
+        <v>4.9306922059999998</v>
+      </c>
+      <c r="E65">
+        <v>4.9739925192282959</v>
       </c>
     </row>
   </sheetData>

</xml_diff>